<commit_message>
400, 703, 705, 784
edited EpiDoc and added translations. The last one (0400) is not yet done.
</commit_message>
<xml_diff>
--- a/alists/EpiDoc.xlsx
+++ b/alists/EpiDoc.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura Löser\OneDrive - Nexus365\Documents\01_Academic\01_Dissertation\Technical\EpiDoc\I.SicilyRepository\ISicily\alists\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_33AE0808DCC105E188F1FBAA6AFF6008C616952E" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -869,8 +875,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,7 +964,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -974,7 +980,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1016,7 +1022,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1049,9 +1055,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1084,6 +1107,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1259,24 +1299,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="100.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="74.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="255.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="100.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.81640625" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" customWidth="1"/>
+    <col min="5" max="5" width="74.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="255.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1296,7 +1336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1312,7 +1352,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1328,7 +1368,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>264</v>
@@ -1344,7 +1384,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1360,7 +1400,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1378,7 +1418,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>20</v>
@@ -1394,7 +1434,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1410,7 +1450,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1428,7 +1468,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1444,7 +1484,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1464,7 +1504,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1480,7 +1520,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -1496,7 +1536,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -1512,7 +1552,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
@@ -1528,7 +1568,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
@@ -1544,7 +1584,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
@@ -1560,7 +1600,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="16.5">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -1576,7 +1616,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>65</v>
@@ -1592,7 +1632,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>69</v>
       </c>
@@ -1608,7 +1648,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
@@ -1624,7 +1664,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>77</v>
       </c>
@@ -1640,7 +1680,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>80</v>
@@ -1652,7 +1692,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
@@ -1668,7 +1708,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>81</v>
       </c>
@@ -1682,7 +1722,7 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>87</v>
       </c>
@@ -1698,7 +1738,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>90</v>
@@ -1712,7 +1752,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>93</v>
@@ -1728,7 +1768,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>97</v>
       </c>
@@ -1744,7 +1784,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>101</v>
       </c>
@@ -1760,7 +1800,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>101</v>
       </c>
@@ -1778,7 +1818,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>107</v>
@@ -1792,7 +1832,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
         <v>110</v>
       </c>
@@ -1808,7 +1848,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
         <v>114</v>
       </c>
@@ -1824,7 +1864,7 @@
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="29">
       <c r="A35" s="1" t="s">
         <v>118</v>
       </c>
@@ -1840,7 +1880,7 @@
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="29">
       <c r="A36" s="1" t="s">
         <v>118</v>
       </c>
@@ -1856,7 +1896,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
         <v>123</v>
       </c>
@@ -1872,7 +1912,7 @@
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
         <v>127</v>
       </c>
@@ -1888,7 +1928,7 @@
       </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
         <v>131</v>
       </c>
@@ -1906,7 +1946,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="29">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>135</v>
@@ -1922,7 +1962,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
         <v>137</v>
       </c>
@@ -1938,7 +1978,7 @@
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>141</v>
@@ -1952,7 +1992,7 @@
       </c>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>144</v>
@@ -1968,7 +2008,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
         <v>148</v>
       </c>
@@ -1984,7 +2024,7 @@
       </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
         <v>152</v>
       </c>
@@ -2000,7 +2040,7 @@
       </c>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
         <v>156</v>
@@ -2016,7 +2056,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
         <v>159</v>
       </c>
@@ -2032,7 +2072,7 @@
       </c>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="29">
       <c r="A48" s="1" t="s">
         <v>162</v>
       </c>
@@ -2048,7 +2088,7 @@
       </c>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="29">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
         <v>165</v>
@@ -2064,7 +2104,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
         <v>168</v>
       </c>
@@ -2080,7 +2120,7 @@
       </c>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="1" t="s">
         <v>171</v>
       </c>
@@ -2096,7 +2136,7 @@
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
@@ -2108,7 +2148,7 @@
       </c>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
@@ -2120,7 +2160,7 @@
       </c>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
         <v>176</v>
       </c>
@@ -2136,7 +2176,7 @@
       </c>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
         <v>179</v>
       </c>
@@ -2154,7 +2194,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
         <v>45</v>
       </c>
@@ -2172,7 +2212,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
         <v>45</v>
       </c>
@@ -2190,7 +2230,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
@@ -2204,7 +2244,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
@@ -2216,7 +2256,7 @@
       </c>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
@@ -2228,14 +2268,14 @@
       </c>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6">
       <c r="A62" s="4" t="s">
         <v>45</v>
       </c>
@@ -2251,7 +2291,7 @@
       </c>
       <c r="F62" s="4"/>
     </row>
-    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6">
       <c r="A63" s="4" t="s">
         <v>45</v>
       </c>
@@ -2269,7 +2309,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6">
       <c r="A64" s="4" t="s">
         <v>45</v>
       </c>
@@ -2287,7 +2327,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6">
       <c r="A65" s="4"/>
       <c r="B65" s="4" t="s">
         <v>240</v>
@@ -2299,7 +2339,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" ht="28.5">
       <c r="A66" s="4" t="s">
         <v>45</v>
       </c>
@@ -2317,7 +2357,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" ht="28.5">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
@@ -2331,7 +2371,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" ht="28.5">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
@@ -2345,7 +2385,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="28.5">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
@@ -2359,7 +2399,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4" t="s">
@@ -2373,7 +2413,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
@@ -2385,7 +2425,7 @@
       </c>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4" t="s">
@@ -2399,7 +2439,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4" t="s">
@@ -2411,7 +2451,7 @@
       </c>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6">
       <c r="A74" s="4" t="s">
         <v>45</v>
       </c>
@@ -2429,7 +2469,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6">
       <c r="A75" s="4" t="s">
         <v>45</v>
       </c>
@@ -2447,7 +2487,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6">
       <c r="A76" s="4" t="s">
         <v>45</v>
       </c>
@@ -2465,7 +2505,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4" t="s">
@@ -2475,7 +2515,7 @@
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2483,7 +2523,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2491,7 +2531,7 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2499,7 +2539,7 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2507,7 +2547,7 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2515,7 +2555,7 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2523,7 +2563,7 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2531,7 +2571,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2539,7 +2579,7 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2547,7 +2587,7 @@
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2555,7 +2595,7 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2563,7 +2603,7 @@
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2578,24 +2618,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>